<commit_message>
Corrección de relación entre entidades y usuario
</commit_message>
<xml_diff>
--- a/Resources/Base de Datos_Proyecto HH_ADFE.xlsx
+++ b/Resources/Base de Datos_Proyecto HH_ADFE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Documents\UMAD\Primavera 2022\Acceso a Datos con Front Ends\ADF_Proyecto_Final\HH_Proyecto\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122657EA-8DF7-44DE-9710-E4639C14B20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4064492A-2141-445D-B588-1A0E837F79F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BA5D8593-2373-472D-BE06-8DE89619F99D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Final_Project</t>
   </si>
@@ -93,9 +93,6 @@
     <t>WQ_1</t>
   </si>
   <si>
-    <t>userId</t>
-  </si>
-  <si>
     <t>startingTime</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>finalGrade</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -283,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,6 +313,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,68 +337,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>30692</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>137584</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>10584</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>102658</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Conector recto de flecha 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8635806-2A0A-427F-97F4-B4DD5D7E27F5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5142442" y="2497667"/>
-          <a:ext cx="307975" cy="166158"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>10584</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -442,13 +392,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1100666</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -495,13 +445,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1100666</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -548,13 +498,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>10583</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>21167</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>116416</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -601,13 +551,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1111250</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>169333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>306917</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>52916</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -658,10 +608,10 @@
       <xdr:rowOff>105834</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>10583</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>312964</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -676,8 +626,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6805083" y="687917"/>
-          <a:ext cx="338667" cy="1397000"/>
+          <a:off x="6381750" y="690941"/>
+          <a:ext cx="312964" cy="2248202"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -705,16 +655,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>6513</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>74084</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1183822</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>21167</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>139211</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>299357</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -728,9 +678,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3541346" y="846667"/>
-          <a:ext cx="1919654" cy="266211"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3510643" y="1115786"/>
+          <a:ext cx="1809750" cy="707571"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -759,15 +709,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>13607</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>232834</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>148166</xdr:rowOff>
+      <xdr:colOff>231322</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -781,9 +731,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3553883" y="1116542"/>
-          <a:ext cx="213784" cy="1783291"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3565071" y="1143000"/>
+          <a:ext cx="217715" cy="3116036"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -812,15 +762,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>21167</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>116417</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -834,9 +784,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3544358" y="1107017"/>
-          <a:ext cx="255059" cy="575733"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3551464" y="1088571"/>
+          <a:ext cx="244929" cy="1551215"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -890,6 +840,59 @@
         <a:xfrm>
           <a:off x="1989667" y="1270000"/>
           <a:ext cx="317500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>65013</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>40822</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Conector recto de flecha 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6D1EEFA-C279-4359-810B-B08EB21E8F41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5034643" y="3249084"/>
+          <a:ext cx="353786" cy="111880"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1215,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DE09B2-BDEF-4E02-AD8E-CCD525C6FD31}">
-  <dimension ref="C1:U25"/>
+  <dimension ref="C1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,13 +1229,13 @@
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1"/>
     <col min="11" max="11" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
@@ -1267,7 +1270,7 @@
       <c r="G3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1280,7 +1283,7 @@
       <c r="F4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1290,14 +1293,14 @@
     <row r="5" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="1"/>
       <c r="F5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1307,19 +1310,19 @@
     </row>
     <row r="6" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1329,24 +1332,24 @@
     </row>
     <row r="7" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="K7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1355,192 +1358,138 @@
     </row>
     <row r="8" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="3" t="s">
-        <v>46</v>
+      <c r="F8" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="1"/>
     </row>
     <row r="9" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="F9" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C10" s="5"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="1"/>
-      <c r="Q10" s="9"/>
       <c r="R10" s="10"/>
       <c r="U10" s="10"/>
     </row>
     <row r="11" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E11" s="1"/>
-      <c r="F11" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="G11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="3" t="str">
-        <f>J4</f>
-        <v>teacherId</v>
-      </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
       <c r="R11" s="10"/>
       <c r="U11" s="10"/>
     </row>
     <row r="12" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="J12" s="5" t="s">
-        <v>26</v>
+      <c r="H12" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="3" t="s">
-        <v>30</v>
+      <c r="L12" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="5" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="5" t="s">
-        <v>24</v>
+      <c r="H13" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="3" t="str">
-        <f>N9</f>
-        <v>frequencyId</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>9</v>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="4" t="s">
-        <v>21</v>
+      <c r="H14" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="3" t="str">
-        <f>N13</f>
-        <v>scheduleId</v>
-      </c>
-      <c r="M14" s="1"/>
-      <c r="N14" s="3" t="s">
-        <v>20</v>
+      <c r="L14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="O14" s="1"/>
+      <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="3" t="s">
-        <v>19</v>
+      <c r="H15" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="3" t="str">
-        <f>N18</f>
-        <v>programId</v>
+        <f>J4</f>
+        <v>teacherId</v>
       </c>
       <c r="M15" s="1"/>
-      <c r="N15" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1548,38 +1497,47 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="2" t="s">
-        <v>16</v>
+      <c r="H16" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="3" t="s">
-        <v>15</v>
+      <c r="J16" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="K16" s="1"/>
-      <c r="L16" s="2" t="str">
-        <f>N22</f>
-        <v>periodId</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N16" s="1"/>
+      <c r="L16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
+      <c r="H17" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="5" t="s">
-        <v>13</v>
+      <c r="J17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="3" t="str">
+        <f>N13</f>
+        <v>frequencyId</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="O17" s="1"/>
     </row>
@@ -1588,16 +1546,21 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="3" t="str">
+        <f>N17</f>
+        <v>scheduleId</v>
+      </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="4" t="s">
-        <v>11</v>
+      <c r="N18" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="O18" s="1"/>
     </row>
@@ -1605,33 +1568,43 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="L19" s="3" t="str">
+        <f>N22</f>
+        <v>programId</v>
+      </c>
+      <c r="M19" s="1"/>
       <c r="N19" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="H20" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="L20" s="2" t="str">
+        <f>N26</f>
+        <v>periodId</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
@@ -1639,16 +1612,18 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="O21" s="1"/>
     </row>
@@ -1656,16 +1631,18 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="H22" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="4" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="O22" s="1"/>
     </row>
@@ -1673,16 +1650,20 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="H23" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="M23" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="N23" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O23" s="1"/>
     </row>
@@ -1690,10 +1671,9 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1707,14 +1687,60 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="2" t="s">
-        <v>50</v>
+      <c r="J25" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+      <c r="N25" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="J26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="J28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modificación del archivo de Excel
</commit_message>
<xml_diff>
--- a/Resources/Base de Datos_Proyecto HH_ADFE.xlsx
+++ b/Resources/Base de Datos_Proyecto HH_ADFE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Documents\UMAD\Primavera 2022\Acceso a Datos con Front Ends\ADF_Proyecto_Final\HH_Proyecto\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4064492A-2141-445D-B588-1A0E837F79F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1539D851-C5F4-4BD6-99B9-DA52D0E2E870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BA5D8593-2373-472D-BE06-8DE89619F99D}"/>
   </bookViews>
@@ -193,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +209,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bahnschrift"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Bahnschrift"/>
@@ -283,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,6 +321,9 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1220,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DE09B2-BDEF-4E02-AD8E-CCD525C6FD31}">
   <dimension ref="C1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,7 +1453,7 @@
       <c r="L13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="N13" s="12" t="s">
         <v>38</v>
       </c>
       <c r="O13" s="1"/>
@@ -1744,6 +1754,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>